<commit_message>
Added function makeAssemblyList(), createAssembly(), createSinglePart() - create parts list recursively.
</commit_message>
<xml_diff>
--- a/test_files/Przykładowy szablon.xlsx
+++ b/test_files/Przykładowy szablon.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="114">
   <si>
     <t>Rodzaj</t>
   </si>
@@ -171,21 +171,9 @@
     <t>2.7</t>
   </si>
   <si>
-    <t>PZP-21.02.11.00-26</t>
-  </si>
-  <si>
-    <t>Blacha 10x730x1000</t>
-  </si>
-  <si>
     <t>2.8</t>
   </si>
   <si>
-    <t>PZP-21.02.12.00-61</t>
-  </si>
-  <si>
-    <t>Blacha 30x150x420</t>
-  </si>
-  <si>
     <t>Grubość</t>
   </si>
   <si>
@@ -346,6 +334,33 @@
   </si>
   <si>
     <t>Koniec</t>
+  </si>
+  <si>
+    <t>2.7.1</t>
+  </si>
+  <si>
+    <t>2.7.2</t>
+  </si>
+  <si>
+    <t>2.7.3</t>
+  </si>
+  <si>
+    <t>2.7.4</t>
+  </si>
+  <si>
+    <t>2.7.5</t>
+  </si>
+  <si>
+    <t>2.7.6</t>
+  </si>
+  <si>
+    <t>2.7.7</t>
+  </si>
+  <si>
+    <t>2.7.8</t>
+  </si>
+  <si>
+    <t>2.9</t>
   </si>
 </sst>
 </file>
@@ -892,6 +907,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -915,9 +933,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1249,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S49"/>
+  <dimension ref="A1:S54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1282,10 +1297,10 @@
       <c r="F1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="46"/>
+      <c r="H1" s="47"/>
       <c r="I1" s="14" t="s">
         <v>18</v>
       </c>
@@ -1308,11 +1323,11 @@
       <c r="D2" s="10"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="49"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="15"/>
@@ -1359,12 +1374,12 @@
       <c r="C4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="49">
-        <f>H34</f>
+      <c r="D4" s="50">
+        <f>H39</f>
         <v>0</v>
       </c>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
       <c r="G4" s="22" t="s">
         <v>25</v>
       </c>
@@ -1387,15 +1402,15 @@
     <row r="5" spans="1:19" ht="15.75" thickBot="1">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="51"/>
+      <c r="D5" s="52"/>
       <c r="E5" s="24"/>
-      <c r="F5" s="52" t="s">
+      <c r="F5" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="53"/>
+      <c r="G5" s="54"/>
       <c r="H5" s="22"/>
       <c r="I5" s="25"/>
       <c r="J5" s="10"/>
@@ -1408,7 +1423,7 @@
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
     </row>
-    <row r="6" spans="1:19" ht="63.75" thickBot="1">
+    <row r="6" spans="1:19" ht="65.25" thickBot="1">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1440,10 +1455,10 @@
         <v>9</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>11</v>
@@ -1455,26 +1470,26 @@
         <v>13</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="Q6" s="6"/>
       <c r="R6" s="5"/>
-      <c r="S6" s="54" t="s">
-        <v>108</v>
+      <c r="S6" s="46" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E7" s="34">
         <v>1</v>
@@ -1498,7 +1513,7 @@
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
@@ -1511,13 +1526,13 @@
         <v>29</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E8" s="28">
         <v>2</v>
@@ -1539,7 +1554,7 @@
       <c r="N8" s="8"/>
       <c r="O8" s="8"/>
       <c r="P8" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
@@ -1552,10 +1567,10 @@
         <v>35</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E9" s="28">
         <v>2</v>
@@ -1570,10 +1585,10 @@
         <v>34</v>
       </c>
       <c r="K9" s="8">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
@@ -1590,10 +1605,10 @@
         <v>38</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E10" s="28">
         <v>1</v>
@@ -1612,11 +1627,11 @@
       </c>
       <c r="L10" s="8"/>
       <c r="M10" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="P10" s="8"/>
       <c r="Q10" s="8"/>
@@ -1630,10 +1645,10 @@
         <v>41</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E11" s="28">
         <v>1</v>
@@ -1653,7 +1668,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
@@ -1691,7 +1706,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
@@ -1703,7 +1718,7 @@
         <v>29</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>36</v>
@@ -1729,7 +1744,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
@@ -1738,27 +1753,32 @@
     </row>
     <row r="14" spans="1:19">
       <c r="A14" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="28">
-        <v>10</v>
-      </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="34">
+        <v>1</v>
+      </c>
+      <c r="F14" s="35">
+        <v>893.21</v>
+      </c>
+      <c r="G14" s="35">
+        <f>F14*E14</f>
+        <v>893.21</v>
+      </c>
+      <c r="H14" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="30"/>
-      <c r="J14" s="31" t="s">
+      <c r="I14" s="36"/>
+      <c r="J14" s="37" t="s">
         <v>34</v>
       </c>
       <c r="K14" s="8">
@@ -1766,7 +1786,7 @@
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="N14" s="8"/>
       <c r="O14" s="8"/>
@@ -1779,13 +1799,13 @@
         <v>29</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="E15" s="28">
         <v>2</v>
@@ -1804,11 +1824,11 @@
       </c>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
-      <c r="N15" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="N15" s="8"/>
       <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
+      <c r="P15" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
     </row>
@@ -1817,16 +1837,16 @@
         <v>29</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="E16" s="28">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F16" s="29"/>
       <c r="G16" s="29"/>
@@ -1840,14 +1860,12 @@
       <c r="K16" s="8">
         <v>30</v>
       </c>
-      <c r="L16" s="8"/>
+      <c r="L16" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="M16" s="8"/>
-      <c r="N16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O16" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
@@ -1857,13 +1875,13 @@
         <v>29</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="C17" s="27" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D17" s="27" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="E17" s="28">
         <v>1</v>
@@ -1878,14 +1896,16 @@
         <v>34</v>
       </c>
       <c r="K17" s="8">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O17" s="8"/>
+      <c r="M17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="P17" s="8"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
@@ -1895,13 +1915,13 @@
         <v>29</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="E18" s="28">
         <v>1</v>
@@ -1918,14 +1938,12 @@
       <c r="K18" s="8">
         <v>30</v>
       </c>
-      <c r="L18" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="L18" s="8"/>
       <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="N18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O18" s="8"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
@@ -1935,13 +1953,13 @@
         <v>29</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>52</v>
+        <v>109</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="E19" s="28">
         <v>2</v>
@@ -1961,7 +1979,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="8"/>
       <c r="N19" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
@@ -1970,43 +1988,38 @@
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="34">
-        <v>7</v>
-      </c>
-      <c r="F20" s="35">
-        <v>627.08000000000004</v>
-      </c>
-      <c r="G20" s="35">
-        <f>F20*E20</f>
-        <v>4389.5600000000004</v>
-      </c>
-      <c r="H20" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="28">
+        <v>10</v>
+      </c>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="37" t="s">
+      <c r="I20" s="30"/>
+      <c r="J20" s="31" t="s">
         <v>34</v>
       </c>
       <c r="K20" s="8">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="N20" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O20" s="8"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
@@ -2016,16 +2029,16 @@
         <v>29</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="C21" s="27" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="E21" s="28">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="29"/>
@@ -2040,10 +2053,10 @@
         <v>30</v>
       </c>
       <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="M21" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" s="8"/>
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
@@ -2054,16 +2067,16 @@
         <v>29</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="E22" s="28">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
@@ -2079,10 +2092,10 @@
       </c>
       <c r="L22" s="8"/>
       <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="N22" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O22" s="8"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
@@ -2092,16 +2105,16 @@
         <v>29</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="E23" s="28">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
@@ -2118,9 +2131,11 @@
       <c r="L23" s="8"/>
       <c r="M23" s="8"/>
       <c r="N23" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O23" s="8"/>
+        <v>52</v>
+      </c>
+      <c r="O23" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
@@ -2130,16 +2145,16 @@
         <v>29</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="E24" s="28">
-        <v>84</v>
+        <v>1</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
@@ -2151,41 +2166,46 @@
         <v>34</v>
       </c>
       <c r="K24" s="8">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="L24" s="8"/>
       <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="N24" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O24" s="8"/>
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
     </row>
     <row r="25" spans="1:18">
       <c r="A25" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="28">
+        <v>53</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="34">
         <v>7</v>
       </c>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="27" t="s">
+      <c r="F25" s="35">
+        <v>627.08000000000004</v>
+      </c>
+      <c r="G25" s="35">
+        <f>F25*E25</f>
+        <v>4389.5600000000004</v>
+      </c>
+      <c r="H25" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="I25" s="30"/>
-      <c r="J25" s="31" t="s">
+      <c r="I25" s="36"/>
+      <c r="J25" s="37" t="s">
         <v>34</v>
       </c>
       <c r="K25" s="8">
@@ -2193,10 +2213,10 @@
       </c>
       <c r="L25" s="8"/>
       <c r="M25" s="8"/>
-      <c r="N25" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
@@ -2206,16 +2226,16 @@
         <v>29</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="E26" s="28">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="F26" s="29"/>
       <c r="G26" s="29"/>
@@ -2231,29 +2251,29 @@
       </c>
       <c r="L26" s="8"/>
       <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="N26" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O26" s="8"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
     </row>
-    <row r="27" spans="1:18" ht="15.75" thickBot="1">
+    <row r="27" spans="1:18">
       <c r="A27" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E27" s="28">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="F27" s="29"/>
       <c r="G27" s="29"/>
@@ -2269,175 +2289,365 @@
       </c>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
-      <c r="N27" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="O27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
     </row>
-    <row r="28" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A28" s="10"/>
-      <c r="B28" s="38"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="42" t="s">
+    <row r="28" spans="1:18">
+      <c r="A28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" s="28">
+        <v>14</v>
+      </c>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="I28" s="30"/>
+      <c r="J28" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28" s="8">
+        <v>30</v>
+      </c>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="28">
+        <v>84</v>
+      </c>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="30"/>
+      <c r="J29" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" s="8">
+        <v>30</v>
+      </c>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="28">
+        <v>7</v>
+      </c>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" s="30"/>
+      <c r="J30" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" s="8">
+        <v>20</v>
+      </c>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8"/>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="28">
+        <v>42</v>
+      </c>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="I31" s="30"/>
+      <c r="J31" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K31" s="8">
+        <v>30</v>
+      </c>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A32" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="28">
+        <v>84</v>
+      </c>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="I32" s="30"/>
+      <c r="J32" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32" s="8">
+        <v>30</v>
+      </c>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8"/>
+    </row>
+    <row r="33" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A33" s="10"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="43">
-        <f>SUM(G6:G27)</f>
-        <v>5282.77</v>
-      </c>
-      <c r="H28" s="44"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-    </row>
-    <row r="32" spans="1:18">
-      <c r="C32" s="45" t="s">
+      <c r="G33" s="43">
+        <f>SUM(G6:G32)</f>
+        <v>6175.9800000000005</v>
+      </c>
+      <c r="H33" s="44"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="15"/>
+      <c r="P33" s="15"/>
+      <c r="Q33" s="15"/>
+      <c r="R33" s="15"/>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="C37" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="D32" s="45" t="s">
+      <c r="E37" s="45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="C38" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E38" s="45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="C39" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="C40" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="C41" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="E41" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="E32" s="45" t="s">
+    </row>
+    <row r="42" spans="1:18">
+      <c r="C42" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="D42" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" s="45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="C46" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="D46" s="45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="C47" s="45" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="33" spans="3:5">
-      <c r="C33" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="D33" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="E33" s="45" t="s">
+      <c r="D47" s="45" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="3:5">
-      <c r="C34" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="45" t="s">
+    <row r="48" spans="1:18">
+      <c r="C48" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="D48" s="45" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="3:5">
-      <c r="C35" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="45" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="3:5">
-      <c r="C36" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="E36" s="45" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5">
-      <c r="C37" s="45" t="s">
-        <v>104</v>
-      </c>
-      <c r="D37" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="E37" s="45" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="3:5">
-      <c r="C41" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="D41" s="45" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="3:5">
-      <c r="C42" s="45" t="s">
-        <v>95</v>
-      </c>
-      <c r="D42" s="45" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="3:5">
-      <c r="C43" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="D43" s="45" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="3:5">
-      <c r="C44" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="D44" s="45" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="45" spans="3:5">
-      <c r="C45" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" s="45" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="46" spans="3:5">
-      <c r="C46" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="D46" s="45" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="3:5">
-      <c r="C47" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="D47" s="45" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="3:5">
-      <c r="C48" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="D48" s="45" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="49" spans="3:4">
       <c r="C49" s="45" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D49" s="45" t="s">
-        <v>100</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4">
+      <c r="C50" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4">
+      <c r="C51" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4">
+      <c r="C52" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="D52" s="45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4">
+      <c r="C53" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="D53" s="45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4">
+      <c r="C54" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="D54" s="45" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>